<commit_message>
#1111 | updating scripts to create relation from test to test_section and unit of measure
</commit_message>
<xml_diff>
--- a/data_migration/lab_data.xlsx
+++ b/data_migration/lab_data.xlsx
@@ -22,7 +22,7 @@
     <t>GROUP / Department</t>
   </si>
   <si>
-    <t>Sample TYPE </t>
+    <t>Sample TYPE</t>
   </si>
   <si>
     <t>PANEL</t>
@@ -31,10 +31,10 @@
     <t>TEST</t>
   </si>
   <si>
-    <t>Short CODE </t>
-  </si>
-  <si>
-    <t>unit </t>
+    <t>Short CODE</t>
+  </si>
+  <si>
+    <t>unit</t>
   </si>
   <si>
     <t>Lower Limit</t>
@@ -105,7 +105,7 @@
     <t>45-55</t>
   </si>
   <si>
-    <t>(later) </t>
+    <t>(later)</t>
   </si>
   <si>
     <t>2 hr</t>
@@ -519,13 +519,13 @@
     <t>0TO 5 CELLS</t>
   </si>
   <si>
-    <t>DLC </t>
+    <t>DLC</t>
   </si>
   <si>
     <t>all mononuciear</t>
   </si>
   <si>
-    <t>BIOCHEMISTRY:</t>
+    <t>BIOCHEMISTRY</t>
   </si>
   <si>
     <t>serum</t>
@@ -1003,7 +1003,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
@@ -1025,10 +1025,6 @@
       <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="false" applyBorder="true" applyFont="false" applyProtection="false" borderId="1" fillId="3" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -1056,7 +1052,7 @@
   <dimension ref="A1:P118"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="H68" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="K94" activeCellId="0" pane="topLeft" sqref="K94"/>
+      <selection activeCell="K94" activeCellId="1" pane="topLeft" sqref="A50:A89 K94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.3"/>
@@ -1984,7 +1980,7 @@
       <c r="O22" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="P22" s="6" t="n">
+      <c r="P22" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2034,7 +2030,7 @@
       <c r="O23" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="P23" s="6" t="n">
+      <c r="P23" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2076,7 +2072,7 @@
       <c r="O24" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="P24" s="6" t="n">
+      <c r="P24" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2118,7 +2114,7 @@
       <c r="O25" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="P25" s="6" t="n">
+      <c r="P25" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2168,7 +2164,7 @@
       <c r="O26" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="P26" s="6" t="n">
+      <c r="P26" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2218,7 +2214,7 @@
       <c r="O27" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="P27" s="6" t="n">
+      <c r="P27" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2260,7 +2256,7 @@
       <c r="O28" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="P28" s="6" t="n">
+      <c r="P28" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2302,7 +2298,7 @@
       <c r="O29" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="P29" s="6" t="n">
+      <c r="P29" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2342,7 +2338,7 @@
       <c r="O30" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="P30" s="6" t="n">
+      <c r="P30" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2384,7 +2380,7 @@
       <c r="O31" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="P31" s="6" t="n">
+      <c r="P31" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2426,7 +2422,7 @@
       <c r="O32" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="P32" s="6" t="n">
+      <c r="P32" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2468,7 +2464,7 @@
       <c r="O33" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="P33" s="6" t="n">
+      <c r="P33" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2510,7 +2506,7 @@
       <c r="O34" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="P34" s="6" t="n">
+      <c r="P34" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2552,7 +2548,7 @@
       <c r="O35" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="P35" s="6" t="n">
+      <c r="P35" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2594,7 +2590,7 @@
       <c r="O36" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="P36" s="6" t="n">
+      <c r="P36" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2636,7 +2632,7 @@
       <c r="O37" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="P37" s="6" t="n">
+      <c r="P37" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2676,7 +2672,7 @@
       <c r="O38" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="P38" s="6" t="n">
+      <c r="P38" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2718,7 +2714,7 @@
       <c r="O39" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="P39" s="6" t="n">
+      <c r="P39" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2768,7 +2764,7 @@
       <c r="O40" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="P40" s="6" t="n">
+      <c r="P40" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2810,7 +2806,7 @@
       <c r="O41" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="P41" s="6" t="n">
+      <c r="P41" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2852,7 +2848,7 @@
       <c r="O42" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="P42" s="6" t="n">
+      <c r="P42" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2894,7 +2890,7 @@
       <c r="O43" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="P43" s="6" t="n">
+      <c r="P43" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2936,7 +2932,7 @@
       <c r="O44" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="P44" s="6" t="n">
+      <c r="P44" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2982,7 +2978,7 @@
       <c r="O45" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="P45" s="6" t="n">
+      <c r="P45" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3024,7 +3020,7 @@
       <c r="O46" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="P46" s="6" t="n">
+      <c r="P46" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3066,7 +3062,7 @@
       <c r="O47" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="P47" s="6" t="n">
+      <c r="P47" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3112,7 +3108,7 @@
       <c r="O48" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="P48" s="7" t="n">
+      <c r="P48" s="6" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3150,7 +3146,7 @@
       <c r="O49" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="P49" s="6" t="n">
+      <c r="P49" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3200,7 +3196,7 @@
       <c r="O50" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="P50" s="6" t="n">
+      <c r="P50" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3250,7 +3246,7 @@
       <c r="O51" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="P51" s="6" t="n">
+      <c r="P51" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3296,7 +3292,7 @@
       <c r="O52" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="P52" s="7"/>
+      <c r="P52" s="6"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.1" outlineLevel="0" r="53">
       <c r="A53" s="3" t="s">
@@ -3344,7 +3340,7 @@
       <c r="O53" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="P53" s="6" t="n">
+      <c r="P53" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3394,7 +3390,7 @@
       <c r="O54" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="P54" s="6" t="n">
+      <c r="P54" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3491,7 +3487,7 @@
       <c r="O56" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="P56" s="6" t="n">
+      <c r="P56" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3541,7 +3537,7 @@
       <c r="O57" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="P57" s="6" t="n">
+      <c r="P57" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3591,7 +3587,7 @@
       <c r="O58" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="P58" s="6" t="n">
+      <c r="P58" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3633,7 +3629,7 @@
       <c r="O59" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="P59" s="7" t="n">
+      <c r="P59" s="6" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3683,7 +3679,7 @@
       <c r="O60" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="P60" s="6" t="n">
+      <c r="P60" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3733,7 +3729,7 @@
       <c r="O61" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="P61" s="6" t="n">
+      <c r="P61" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3775,7 +3771,7 @@
       <c r="O62" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="P62" s="7" t="n">
+      <c r="P62" s="6" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3825,7 +3821,7 @@
       <c r="O63" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="P63" s="6" t="n">
+      <c r="P63" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3871,7 +3867,7 @@
       <c r="O64" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="P64" s="6" t="n">
+      <c r="P64" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3921,7 +3917,7 @@
       <c r="O65" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="P65" s="6" t="n">
+      <c r="P65" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3963,7 +3959,7 @@
       <c r="O66" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="P66" s="7" t="n">
+      <c r="P66" s="6" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4013,7 +4009,7 @@
       <c r="O67" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="P67" s="6" t="n">
+      <c r="P67" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4063,7 +4059,7 @@
       <c r="O68" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="P68" s="6" t="n">
+      <c r="P68" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4113,7 +4109,7 @@
       <c r="O69" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="P69" s="6" t="n">
+      <c r="P69" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4163,7 +4159,7 @@
       <c r="O70" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="P70" s="6" t="n">
+      <c r="P70" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4203,7 +4199,7 @@
       <c r="O71" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="P71" s="6" t="n">
+      <c r="P71" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4253,7 +4249,7 @@
       <c r="O72" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="P72" s="6" t="n">
+      <c r="P72" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4303,7 +4299,7 @@
       <c r="O73" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="P73" s="6" t="n">
+      <c r="P73" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4353,7 +4349,7 @@
       <c r="O74" s="3" t="s">
         <v>246</v>
       </c>
-      <c r="P74" s="6" t="n">
+      <c r="P74" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4403,7 +4399,7 @@
       <c r="O75" s="3" t="s">
         <v>250</v>
       </c>
-      <c r="P75" s="6" t="n">
+      <c r="P75" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4453,7 +4449,7 @@
       <c r="O76" s="3" t="s">
         <v>250</v>
       </c>
-      <c r="P76" s="6" t="n">
+      <c r="P76" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4503,7 +4499,7 @@
       <c r="O77" s="3" t="s">
         <v>250</v>
       </c>
-      <c r="P77" s="6" t="n">
+      <c r="P77" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4553,7 +4549,7 @@
       <c r="O78" s="3" t="s">
         <v>250</v>
       </c>
-      <c r="P78" s="6" t="n">
+      <c r="P78" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4603,7 +4599,7 @@
       <c r="O79" s="3" t="s">
         <v>250</v>
       </c>
-      <c r="P79" s="6" t="n">
+      <c r="P79" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4653,7 +4649,7 @@
       <c r="O80" s="3" t="s">
         <v>250</v>
       </c>
-      <c r="P80" s="6" t="n">
+      <c r="P80" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4703,7 +4699,7 @@
       <c r="O81" s="3" t="s">
         <v>250</v>
       </c>
-      <c r="P81" s="6" t="n">
+      <c r="P81" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4753,7 +4749,7 @@
       <c r="O82" s="3" t="s">
         <v>250</v>
       </c>
-      <c r="P82" s="6" t="n">
+      <c r="P82" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4803,7 +4799,7 @@
       <c r="O83" s="3" t="s">
         <v>250</v>
       </c>
-      <c r="P83" s="6" t="n">
+      <c r="P83" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4845,7 +4841,7 @@
       <c r="O84" s="4" t="s">
         <v>250</v>
       </c>
-      <c r="P84" s="7" t="n">
+      <c r="P84" s="6" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4891,7 +4887,7 @@
       <c r="O85" s="3" t="s">
         <v>250</v>
       </c>
-      <c r="P85" s="6" t="n">
+      <c r="P85" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4937,278 +4933,270 @@
       <c r="O86" s="3" t="s">
         <v>250</v>
       </c>
-      <c r="P86" s="6" t="n">
+      <c r="P86" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.1" outlineLevel="0" r="87">
-      <c r="A87" s="6" t="s">
+      <c r="A87" s="0" t="s">
         <v>168</v>
       </c>
-      <c r="B87" s="6" t="s">
+      <c r="B87" s="0" t="s">
         <v>169</v>
       </c>
-      <c r="C87" s="6" t="s">
+      <c r="C87" s="0" t="s">
         <v>258</v>
       </c>
-      <c r="D87" s="6" t="s">
+      <c r="D87" s="0" t="s">
         <v>288</v>
       </c>
-      <c r="E87" s="6" t="s">
+      <c r="E87" s="0" t="s">
         <v>288</v>
       </c>
-      <c r="F87" s="6" t="s">
+      <c r="F87" s="0" t="s">
         <v>285</v>
       </c>
-      <c r="G87" s="6"/>
-      <c r="H87" s="6"/>
-      <c r="I87" s="6" t="s">
+      <c r="I87" s="0" t="s">
         <v>236</v>
       </c>
-      <c r="J87" s="6"/>
-      <c r="K87" s="6"/>
-      <c r="L87" s="6" t="s">
+      <c r="L87" s="0" t="s">
         <v>236</v>
       </c>
-      <c r="M87" s="6" t="n">
+      <c r="M87" s="0" t="n">
         <v>400</v>
       </c>
-      <c r="N87" s="6" t="s">
+      <c r="N87" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="O87" s="6" t="s">
+      <c r="O87" s="0" t="s">
         <v>250</v>
       </c>
-      <c r="P87" s="6" t="n">
+      <c r="P87" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.1" outlineLevel="0" r="88">
-      <c r="A88" s="7" t="s">
+      <c r="A88" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="B88" s="7" t="s">
+      <c r="B88" s="6" t="s">
         <v>169</v>
       </c>
-      <c r="C88" s="7" t="s">
+      <c r="C88" s="6" t="s">
         <v>258</v>
       </c>
-      <c r="D88" s="7" t="s">
+      <c r="D88" s="6" t="s">
         <v>289</v>
       </c>
-      <c r="E88" s="7" t="s">
+      <c r="E88" s="6" t="s">
         <v>289</v>
       </c>
-      <c r="F88" s="7" t="s">
+      <c r="F88" s="6" t="s">
         <v>290</v>
       </c>
-      <c r="G88" s="7"/>
-      <c r="H88" s="7"/>
-      <c r="I88" s="7" t="s">
+      <c r="G88" s="6"/>
+      <c r="H88" s="6"/>
+      <c r="I88" s="6" t="s">
         <v>291</v>
       </c>
-      <c r="J88" s="7"/>
-      <c r="K88" s="7"/>
-      <c r="L88" s="7" t="s">
+      <c r="J88" s="6"/>
+      <c r="K88" s="6"/>
+      <c r="L88" s="6" t="s">
         <v>236</v>
       </c>
-      <c r="M88" s="7" t="n">
+      <c r="M88" s="6" t="n">
         <v>400</v>
       </c>
-      <c r="N88" s="7" t="s">
+      <c r="N88" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="O88" s="7" t="s">
+      <c r="O88" s="6" t="s">
         <v>250</v>
       </c>
-      <c r="P88" s="7" t="n">
+      <c r="P88" s="6" t="n">
         <v>0</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="89">
-      <c r="A89" s="6" t="s">
+      <c r="A89" s="0" t="s">
         <v>168</v>
       </c>
-      <c r="B89" s="6" t="s">
+      <c r="B89" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="C89" s="6" t="s">
+      <c r="C89" s="0" t="s">
         <v>292</v>
       </c>
-      <c r="D89" s="6" t="s">
+      <c r="D89" s="0" t="s">
         <v>293</v>
       </c>
-      <c r="E89" s="6" t="s">
+      <c r="E89" s="0" t="s">
         <v>293</v>
       </c>
-      <c r="F89" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="G89" s="6"/>
-      <c r="H89" s="6"/>
-      <c r="I89" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="J89" s="6"/>
-      <c r="K89" s="6"/>
-      <c r="L89" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="M89" s="6" t="n">
+      <c r="F89" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="I89" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="L89" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="M89" s="0" t="n">
         <v>500</v>
       </c>
-      <c r="N89" s="6" t="s">
+      <c r="N89" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="O89" s="6" t="s">
+      <c r="O89" s="0" t="s">
         <v>250</v>
       </c>
-      <c r="P89" s="6" t="n">
+      <c r="P89" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="90">
-      <c r="P90" s="6" t="n">
+      <c r="P90" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="91">
-      <c r="P91" s="6" t="n">
+      <c r="P91" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="92">
-      <c r="P92" s="6" t="n">
+      <c r="P92" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="93">
-      <c r="P93" s="6" t="n">
+      <c r="P93" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="94">
-      <c r="P94" s="6" t="n">
+      <c r="P94" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="95">
-      <c r="P95" s="6" t="n">
+      <c r="P95" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="96">
-      <c r="P96" s="6" t="n">
+      <c r="P96" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="97">
-      <c r="P97" s="6" t="n">
+      <c r="P97" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="98">
-      <c r="P98" s="6" t="n">
+      <c r="P98" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="99">
-      <c r="P99" s="6" t="n">
+      <c r="P99" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="100">
-      <c r="P100" s="6" t="n">
+      <c r="P100" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="101">
-      <c r="P101" s="6" t="n">
+      <c r="P101" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="102">
-      <c r="P102" s="6" t="n">
+      <c r="P102" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="103">
-      <c r="P103" s="6" t="n">
+      <c r="P103" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="104">
-      <c r="P104" s="6" t="n">
+      <c r="P104" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="105">
-      <c r="P105" s="6" t="n">
+      <c r="P105" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="106">
-      <c r="P106" s="6" t="n">
+      <c r="P106" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="107">
-      <c r="P107" s="6" t="n">
+      <c r="P107" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="108">
-      <c r="P108" s="6" t="n">
+      <c r="P108" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="109">
-      <c r="P109" s="6" t="n">
+      <c r="P109" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="110">
-      <c r="P110" s="6" t="n">
+      <c r="P110" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="111">
-      <c r="P111" s="6" t="n">
+      <c r="P111" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="112">
-      <c r="P112" s="6" t="n">
+      <c r="P112" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="113">
-      <c r="P113" s="6" t="n">
+      <c r="P113" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="114">
-      <c r="P114" s="6" t="n">
+      <c r="P114" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="115">
-      <c r="P115" s="6" t="n">
+      <c r="P115" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="116">
-      <c r="P116" s="6" t="n">
+      <c r="P116" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="117">
-      <c r="P117" s="6" t="n">
+      <c r="P117" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="118">
-      <c r="P118" s="6" t="n">
+      <c r="P118" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5231,7 +5219,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+      <selection activeCell="A1" activeCellId="1" pane="topLeft" sqref="A50:A89 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
@@ -5257,7 +5245,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+      <selection activeCell="A1" activeCellId="1" pane="topLeft" sqref="A50:A89 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>

</xml_diff>

<commit_message>
Banka | Fixing perl script to escape single quotes in test name         Capitalizing sample type stool to Stool.
</commit_message>
<xml_diff>
--- a/data_migration/lab_data.xlsx
+++ b/data_migration/lab_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16460" tabRatio="480" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16460" tabRatio="480"/>
   </bookViews>
   <sheets>
     <sheet name="lab_data" sheetId="14" r:id="rId1"/>
@@ -1385,9 +1385,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="174">
+  <cellStyleXfs count="178">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1605,6 +1609,7 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1613,9 +1618,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="174">
+  <cellStyles count="178">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -1702,6 +1706,8 @@
     <cellStyle name="Followed Hyperlink" xfId="169" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="171" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="173" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="175" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="177" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -1788,6 +1794,8 @@
     <cellStyle name="Hyperlink" xfId="168" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="170" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="172" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="174" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="176" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -2096,8 +2104,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K244"/>
   <sheetViews>
-    <sheetView topLeftCell="A211" workbookViewId="0">
-      <selection activeCell="A244" sqref="A244"/>
+    <sheetView tabSelected="1" topLeftCell="A217" workbookViewId="0">
+      <selection activeCell="D238" sqref="D238"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -7326,7 +7334,7 @@
         <v>95</v>
       </c>
       <c r="B182" s="28" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C182" s="28" t="s">
         <v>104</v>
@@ -8013,7 +8021,7 @@
         <v>95</v>
       </c>
       <c r="B207" s="28" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C207" s="28" t="s">
         <v>102</v>
@@ -8154,7 +8162,7 @@
         <v>95</v>
       </c>
       <c r="B212" s="28" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C212" s="28" t="s">
         <v>101</v>
@@ -8891,108 +8899,108 @@
       <c r="K238" s="2"/>
     </row>
     <row r="239" spans="1:11">
-      <c r="A239" s="37" t="s">
+      <c r="A239" s="33" t="s">
         <v>236</v>
       </c>
-      <c r="B239" s="37" t="s">
+      <c r="B239" s="33" t="s">
         <v>232</v>
       </c>
-      <c r="C239" s="37"/>
-      <c r="D239" s="37" t="s">
+      <c r="C239" s="33"/>
+      <c r="D239" s="33" t="s">
         <v>225</v>
       </c>
-      <c r="E239" s="37"/>
-      <c r="F239" s="37"/>
-      <c r="G239" s="37" t="s">
+      <c r="E239" s="33"/>
+      <c r="F239" s="33"/>
+      <c r="G239" s="33" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="240" spans="1:11">
-      <c r="A240" s="37" t="s">
+      <c r="A240" s="33" t="s">
         <v>236</v>
       </c>
-      <c r="B240" s="37" t="s">
+      <c r="B240" s="33" t="s">
         <v>95</v>
       </c>
-      <c r="C240" s="37"/>
-      <c r="D240" s="37" t="s">
+      <c r="C240" s="33"/>
+      <c r="D240" s="33" t="s">
         <v>357</v>
       </c>
-      <c r="E240" s="37" t="s">
+      <c r="E240" s="33" t="s">
         <v>225</v>
       </c>
-      <c r="F240" s="37"/>
-      <c r="G240" s="37" t="s">
+      <c r="F240" s="33"/>
+      <c r="G240" s="33" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="241" spans="1:7">
-      <c r="A241" s="37" t="s">
+      <c r="A241" s="33" t="s">
         <v>236</v>
       </c>
-      <c r="B241" s="37" t="s">
+      <c r="B241" s="33" t="s">
         <v>67</v>
       </c>
-      <c r="C241" s="37"/>
-      <c r="D241" s="37" t="s">
+      <c r="C241" s="33"/>
+      <c r="D241" s="33" t="s">
         <v>357</v>
       </c>
-      <c r="E241" s="37" t="s">
+      <c r="E241" s="33" t="s">
         <v>225</v>
       </c>
-      <c r="F241" s="37"/>
-      <c r="G241" s="37" t="s">
+      <c r="F241" s="33"/>
+      <c r="G241" s="33" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="242" spans="1:7">
-      <c r="A242" s="37" t="s">
+      <c r="A242" s="33" t="s">
         <v>236</v>
       </c>
-      <c r="B242" s="37" t="s">
+      <c r="B242" s="33" t="s">
         <v>358</v>
       </c>
-      <c r="C242" s="37"/>
-      <c r="D242" s="37" t="s">
+      <c r="C242" s="33"/>
+      <c r="D242" s="33" t="s">
         <v>225</v>
       </c>
-      <c r="E242" s="37"/>
-      <c r="F242" s="37"/>
-      <c r="G242" s="37" t="s">
+      <c r="E242" s="33"/>
+      <c r="F242" s="33"/>
+      <c r="G242" s="33" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="243" spans="1:7">
-      <c r="A243" s="37" t="s">
+      <c r="A243" s="33" t="s">
         <v>236</v>
       </c>
-      <c r="B243" s="37" t="s">
+      <c r="B243" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="C243" s="37"/>
-      <c r="D243" s="37" t="s">
+      <c r="C243" s="33"/>
+      <c r="D243" s="33" t="s">
         <v>225</v>
       </c>
-      <c r="E243" s="37"/>
-      <c r="F243" s="37"/>
-      <c r="G243" s="37" t="s">
+      <c r="E243" s="33"/>
+      <c r="F243" s="33"/>
+      <c r="G243" s="33" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="244" spans="1:7">
-      <c r="A244" s="37" t="s">
+      <c r="A244" s="33" t="s">
         <v>236</v>
       </c>
-      <c r="B244" s="37" t="s">
+      <c r="B244" s="33" t="s">
         <v>237</v>
       </c>
-      <c r="C244" s="37"/>
-      <c r="D244" s="37" t="s">
+      <c r="C244" s="33"/>
+      <c r="D244" s="33" t="s">
         <v>225</v>
       </c>
-      <c r="E244" s="37"/>
-      <c r="F244" s="37"/>
-      <c r="G244" s="37" t="s">
+      <c r="E244" s="33"/>
+      <c r="F244" s="33"/>
+      <c r="G244" s="33" t="s">
         <v>216</v>
       </c>
     </row>
@@ -9010,8 +9018,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P196"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A172" workbookViewId="0">
-      <selection activeCell="B196" sqref="B196"/>
+    <sheetView topLeftCell="A173" workbookViewId="0">
+      <selection activeCell="D194" sqref="D194"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -10719,7 +10727,7 @@
       <c r="C45" t="s">
         <v>335</v>
       </c>
-      <c r="D45" s="37" t="s">
+      <c r="D45" s="33" t="s">
         <v>358</v>
       </c>
       <c r="G45" t="s">
@@ -16899,10 +16907,10 @@
       <c r="C196" t="s">
         <v>335</v>
       </c>
-      <c r="D196" s="37" t="s">
+      <c r="D196" s="33" t="s">
         <v>357</v>
       </c>
-      <c r="E196" s="37" t="s">
+      <c r="E196" s="33" t="s">
         <v>225</v>
       </c>
       <c r="G196" t="s">
@@ -16932,7 +16940,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -24832,112 +24839,112 @@
       </c>
     </row>
     <row r="239" spans="1:11" ht="14">
-      <c r="A239" s="37" t="s">
+      <c r="A239" s="33" t="s">
         <v>236</v>
       </c>
-      <c r="B239" s="37" t="s">
+      <c r="B239" s="33" t="s">
         <v>232</v>
       </c>
-      <c r="C239" s="37"/>
-      <c r="D239" s="37" t="s">
+      <c r="C239" s="33"/>
+      <c r="D239" s="33" t="s">
         <v>225</v>
       </c>
-      <c r="E239" s="37"/>
-      <c r="F239" s="37"/>
-      <c r="G239" s="37" t="s">
+      <c r="E239" s="33"/>
+      <c r="F239" s="33"/>
+      <c r="G239" s="33" t="s">
         <v>216</v>
       </c>
-      <c r="H239" s="37"/>
-      <c r="I239" s="37"/>
-      <c r="J239" s="37"/>
-      <c r="K239" s="37"/>
+      <c r="H239" s="33"/>
+      <c r="I239" s="33"/>
+      <c r="J239" s="33"/>
+      <c r="K239" s="33"/>
     </row>
     <row r="240" spans="1:11" ht="14">
-      <c r="A240" s="37" t="s">
+      <c r="A240" s="33" t="s">
         <v>236</v>
       </c>
-      <c r="B240" s="37" t="s">
+      <c r="B240" s="33" t="s">
         <v>95</v>
       </c>
-      <c r="C240" s="37"/>
-      <c r="D240" s="37" t="s">
+      <c r="C240" s="33"/>
+      <c r="D240" s="33" t="s">
         <v>357</v>
       </c>
-      <c r="E240" s="37" t="s">
+      <c r="E240" s="33" t="s">
         <v>225</v>
       </c>
-      <c r="F240" s="37"/>
-      <c r="G240" s="37" t="s">
+      <c r="F240" s="33"/>
+      <c r="G240" s="33" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="241" spans="1:7" ht="14">
-      <c r="A241" s="37" t="s">
+      <c r="A241" s="33" t="s">
         <v>236</v>
       </c>
-      <c r="B241" s="37" t="s">
+      <c r="B241" s="33" t="s">
         <v>67</v>
       </c>
-      <c r="C241" s="37"/>
-      <c r="D241" s="37" t="s">
+      <c r="C241" s="33"/>
+      <c r="D241" s="33" t="s">
         <v>357</v>
       </c>
-      <c r="E241" s="37" t="s">
+      <c r="E241" s="33" t="s">
         <v>225</v>
       </c>
-      <c r="F241" s="37"/>
-      <c r="G241" s="37" t="s">
+      <c r="F241" s="33"/>
+      <c r="G241" s="33" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="242" spans="1:7" ht="14">
-      <c r="A242" s="37" t="s">
+      <c r="A242" s="33" t="s">
         <v>236</v>
       </c>
-      <c r="B242" s="37" t="s">
+      <c r="B242" s="33" t="s">
         <v>358</v>
       </c>
-      <c r="C242" s="37"/>
-      <c r="D242" s="37" t="s">
+      <c r="C242" s="33"/>
+      <c r="D242" s="33" t="s">
         <v>225</v>
       </c>
-      <c r="E242" s="37"/>
-      <c r="F242" s="37"/>
-      <c r="G242" s="37" t="s">
+      <c r="E242" s="33"/>
+      <c r="F242" s="33"/>
+      <c r="G242" s="33" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="243" spans="1:7" ht="14">
-      <c r="A243" s="37" t="s">
+      <c r="A243" s="33" t="s">
         <v>236</v>
       </c>
-      <c r="B243" s="37" t="s">
+      <c r="B243" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="C243" s="37"/>
-      <c r="D243" s="37" t="s">
+      <c r="C243" s="33"/>
+      <c r="D243" s="33" t="s">
         <v>225</v>
       </c>
-      <c r="E243" s="37"/>
-      <c r="F243" s="37"/>
-      <c r="G243" s="37" t="s">
+      <c r="E243" s="33"/>
+      <c r="F243" s="33"/>
+      <c r="G243" s="33" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="244" spans="1:7" ht="14">
-      <c r="A244" s="37" t="s">
+      <c r="A244" s="33" t="s">
         <v>236</v>
       </c>
-      <c r="B244" s="37" t="s">
+      <c r="B244" s="33" t="s">
         <v>237</v>
       </c>
-      <c r="C244" s="37"/>
-      <c r="D244" s="37" t="s">
+      <c r="C244" s="33"/>
+      <c r="D244" s="33" t="s">
         <v>225</v>
       </c>
-      <c r="E244" s="37"/>
-      <c r="F244" s="37"/>
-      <c r="G244" s="37" t="s">
+      <c r="E244" s="33"/>
+      <c r="F244" s="33"/>
+      <c r="G244" s="33" t="s">
         <v>216</v>
       </c>
     </row>
@@ -24948,7 +24955,6 @@
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -30118,31 +30124,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="33" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="33" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="33" t="s">
+      <c r="A1" s="34" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="34" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="33" t="s">
+      <c r="D1" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="33" t="s">
+      <c r="E1" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="33" t="s">
+      <c r="F1" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="33" t="s">
+      <c r="G1" s="34" t="s">
         <v>208</v>
       </c>
       <c r="H1" s="25" t="s">
         <v>313</v>
       </c>
-      <c r="I1" s="35" t="s">
+      <c r="I1" s="36" t="s">
         <v>146</v>
       </c>
       <c r="J1" s="25" t="s">
@@ -30153,17 +30159,17 @@
       </c>
     </row>
     <row r="2" spans="1:11">
-      <c r="A2" s="34"/>
-      <c r="B2" s="34"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
+      <c r="A2" s="35"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
       <c r="H2" s="26" t="s">
         <v>314</v>
       </c>
-      <c r="I2" s="36"/>
+      <c r="I2" s="37"/>
       <c r="J2" s="26" t="s">
         <v>314</v>
       </c>

</xml_diff>

<commit_message>
Banka | Change tests & panels.
</commit_message>
<xml_diff>
--- a/data_migration/lab_data.xlsx
+++ b/data_migration/lab_data.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8806" uniqueCount="485">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8806" uniqueCount="517">
   <si>
     <t>GROUP / Department</t>
   </si>
@@ -1644,6 +1644,174 @@
   </si>
   <si>
     <t>Added panel in ERP</t>
+  </si>
+  <si>
+    <r>
+      <t>APTT (Test)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> (Serum)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>APTT (Test)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> (Blood)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>APTT (Control)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> (Serum)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>APTT (Control)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> (Blood)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>INR Ratio</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> (Blood)</t>
+    </r>
+  </si>
+  <si>
+    <t>INR Ratio (Serum)</t>
+  </si>
+  <si>
+    <t>Prothrombin Time (Control) (Blood)</t>
+  </si>
+  <si>
+    <t>Prothrombin Time (Control) (Serum)</t>
+  </si>
+  <si>
+    <t>Prothrombin Time (Test) (Blood)</t>
+  </si>
+  <si>
+    <t>Prothrombin Time (Test) (Serum)</t>
+  </si>
+  <si>
+    <t>Culture (Sputum)</t>
+  </si>
+  <si>
+    <t>Culture (Tissue)</t>
+  </si>
+  <si>
+    <t>Culture (Blood)</t>
+  </si>
+  <si>
+    <t>Culture (Semen)</t>
+  </si>
+  <si>
+    <t>Gram Stain (Semen)</t>
+  </si>
+  <si>
+    <t>Gram Stain (Blood)</t>
+  </si>
+  <si>
+    <t>Gram Stain (Urine)</t>
+  </si>
+  <si>
+    <t>Gram Stain (Stool)</t>
+  </si>
+  <si>
+    <t>Gram Stain (Sputum)</t>
+  </si>
+  <si>
+    <t>Gram Stain (Slit Skin)</t>
+  </si>
+  <si>
+    <t>Gram Stain (Body Fluid)</t>
+  </si>
+  <si>
+    <t>HIV ELISA (Blood)</t>
+  </si>
+  <si>
+    <r>
+      <t>HIV ELISA</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> (Serum)</t>
+    </r>
+  </si>
+  <si>
+    <t>Routine Microbiology Culture (Stool)</t>
+  </si>
+  <si>
+    <t>Routine Microbiology Culture (Urine)</t>
+  </si>
+  <si>
+    <t>ZN Stain (Urine)</t>
+  </si>
+  <si>
+    <t>ZN Stain (Stool)</t>
+  </si>
+  <si>
+    <t>ZN Stain (Sputum)</t>
+  </si>
+  <si>
+    <t>ZN Stain (Body Fluid)</t>
+  </si>
+  <si>
+    <t>ZN Stain (Slit Skin)</t>
+  </si>
+  <si>
+    <t>ZN Stain (Body Fluid) (Pus)</t>
+  </si>
+  <si>
+    <t>Gram Stain (Body Fluid) (Pus)</t>
   </si>
 </sst>
 </file>
@@ -1906,9 +2074,145 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="360">
+  <cellStyleXfs count="496">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2339,6 +2643,10 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2347,12 +2655,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="360">
+  <cellStyles count="496">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -2532,6 +2836,74 @@
     <cellStyle name="Followed Hyperlink" xfId="355" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="357" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="359" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="361" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="363" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="365" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="367" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="369" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="371" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="373" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="375" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="377" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="379" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="381" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="383" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="385" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="387" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="389" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="391" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="393" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="395" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="397" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="399" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="401" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="403" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="405" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="407" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="409" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="411" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="413" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="415" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="417" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="419" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="421" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="423" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="425" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="427" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="429" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="431" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="433" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="435" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="437" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="439" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="441" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="443" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="445" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="447" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="449" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="451" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="453" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="455" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="457" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="459" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="461" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="463" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="465" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="467" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="469" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="471" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="473" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="475" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="477" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="479" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="481" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="483" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="485" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="487" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="489" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="491" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="493" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="495" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -2711,6 +3083,74 @@
     <cellStyle name="Hyperlink" xfId="354" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="356" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="358" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="360" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="362" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="364" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="366" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="368" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="370" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="372" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="374" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="376" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="378" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="380" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="382" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="384" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="386" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="388" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="390" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="392" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="394" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="396" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="398" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="400" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="402" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="404" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="406" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="408" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="410" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="412" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="414" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="416" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="418" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="420" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="422" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="424" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="426" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="428" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="430" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="432" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="434" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="436" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="438" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="440" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="442" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="444" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="446" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="448" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="450" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="452" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="454" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="456" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="458" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="460" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="462" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="464" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="466" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="468" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="470" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="472" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="474" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="476" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="478" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="480" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="482" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="484" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="486" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="488" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="490" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="492" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="494" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -3019,8 +3459,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M277"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A111" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="D131" sqref="D131"/>
+    <sheetView tabSelected="1" topLeftCell="A257" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="D277" sqref="D277"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -3037,37 +3477,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="25">
-      <c r="A1" s="60" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="60" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="60" t="s">
+      <c r="A1" s="56" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="60" t="s">
+      <c r="D1" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="60" t="s">
+      <c r="E1" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="60" t="s">
+      <c r="F1" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="60" t="s">
+      <c r="G1" s="56" t="s">
         <v>208</v>
       </c>
-      <c r="H1" s="61" t="s">
+      <c r="H1" s="57" t="s">
         <v>145</v>
       </c>
-      <c r="I1" s="61" t="s">
+      <c r="I1" s="57" t="s">
         <v>146</v>
       </c>
-      <c r="J1" s="61" t="s">
+      <c r="J1" s="57" t="s">
         <v>147</v>
       </c>
-      <c r="K1" s="61" t="s">
+      <c r="K1" s="57" t="s">
         <v>148</v>
       </c>
     </row>
@@ -3374,8 +3814,8 @@
       <c r="C11" s="18" t="s">
         <v>372</v>
       </c>
-      <c r="D11" s="5" t="s">
-        <v>270</v>
+      <c r="D11" s="18" t="s">
+        <v>487</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>272</v>
@@ -3409,8 +3849,8 @@
       <c r="C12" s="18" t="s">
         <v>262</v>
       </c>
-      <c r="D12" s="5" t="s">
-        <v>270</v>
+      <c r="D12" s="18" t="s">
+        <v>488</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>272</v>
@@ -3444,8 +3884,8 @@
       <c r="C13" s="18" t="s">
         <v>372</v>
       </c>
-      <c r="D13" s="5" t="s">
-        <v>271</v>
+      <c r="D13" s="18" t="s">
+        <v>485</v>
       </c>
       <c r="E13" s="5" t="s">
         <v>273</v>
@@ -3479,8 +3919,8 @@
       <c r="C14" s="18" t="s">
         <v>262</v>
       </c>
-      <c r="D14" s="5" t="s">
-        <v>271</v>
+      <c r="D14" s="18" t="s">
+        <v>486</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>273</v>
@@ -4229,7 +4669,7 @@
       </c>
       <c r="C40" s="34"/>
       <c r="D40" s="40" t="s">
-        <v>225</v>
+        <v>495</v>
       </c>
       <c r="E40" s="34"/>
       <c r="F40" s="34"/>
@@ -4250,7 +4690,7 @@
       </c>
       <c r="C41" s="34"/>
       <c r="D41" s="40" t="s">
-        <v>225</v>
+        <v>496</v>
       </c>
       <c r="E41" s="34"/>
       <c r="F41" s="34"/>
@@ -4271,7 +4711,7 @@
       </c>
       <c r="C42" s="34"/>
       <c r="D42" s="40" t="s">
-        <v>225</v>
+        <v>497</v>
       </c>
       <c r="E42" s="34"/>
       <c r="F42" s="34"/>
@@ -4292,7 +4732,7 @@
       </c>
       <c r="C43" s="34"/>
       <c r="D43" s="40" t="s">
-        <v>225</v>
+        <v>498</v>
       </c>
       <c r="E43" s="34"/>
       <c r="F43" s="34"/>
@@ -5284,7 +5724,7 @@
         <v>238</v>
       </c>
       <c r="D80" s="18" t="s">
-        <v>110</v>
+        <v>499</v>
       </c>
       <c r="E80" s="18"/>
       <c r="F80" s="18"/>
@@ -5305,7 +5745,7 @@
       </c>
       <c r="C81" s="41"/>
       <c r="D81" s="18" t="s">
-        <v>110</v>
+        <v>500</v>
       </c>
       <c r="E81" s="18"/>
       <c r="F81" s="18" t="s">
@@ -5328,7 +5768,7 @@
       </c>
       <c r="C82" s="41"/>
       <c r="D82" s="18" t="s">
-        <v>110</v>
+        <v>501</v>
       </c>
       <c r="E82" s="18"/>
       <c r="F82" s="18" t="s">
@@ -5351,7 +5791,7 @@
       </c>
       <c r="C83" s="41"/>
       <c r="D83" s="18" t="s">
-        <v>110</v>
+        <v>502</v>
       </c>
       <c r="E83" s="18"/>
       <c r="F83" s="18" t="s">
@@ -5374,7 +5814,7 @@
       </c>
       <c r="C84" s="41"/>
       <c r="D84" s="18" t="s">
-        <v>110</v>
+        <v>503</v>
       </c>
       <c r="E84" s="18"/>
       <c r="F84" s="18" t="s">
@@ -5397,7 +5837,7 @@
       </c>
       <c r="C85" s="41"/>
       <c r="D85" s="18" t="s">
-        <v>110</v>
+        <v>505</v>
       </c>
       <c r="E85" s="18"/>
       <c r="F85" s="18" t="s">
@@ -5420,7 +5860,7 @@
       </c>
       <c r="C86" s="41"/>
       <c r="D86" s="18" t="s">
-        <v>110</v>
+        <v>404</v>
       </c>
       <c r="E86" s="18"/>
       <c r="F86" s="18" t="s">
@@ -5443,7 +5883,7 @@
       </c>
       <c r="C87" s="41"/>
       <c r="D87" s="18" t="s">
-        <v>110</v>
+        <v>504</v>
       </c>
       <c r="E87" s="18"/>
       <c r="F87" s="18" t="s">
@@ -5466,7 +5906,7 @@
       </c>
       <c r="C88" s="41"/>
       <c r="D88" s="18" t="s">
-        <v>110</v>
+        <v>499</v>
       </c>
       <c r="E88" s="18"/>
       <c r="F88" s="18" t="s">
@@ -5583,7 +6023,7 @@
         <v>221</v>
       </c>
       <c r="D93" s="19" t="s">
-        <v>404</v>
+        <v>516</v>
       </c>
       <c r="E93" s="18"/>
       <c r="F93" s="18"/>
@@ -6268,7 +6708,7 @@
         <v>255</v>
       </c>
       <c r="D117" s="18" t="s">
-        <v>187</v>
+        <v>506</v>
       </c>
       <c r="E117" s="18"/>
       <c r="F117" s="18" t="s">
@@ -6295,7 +6735,7 @@
         <v>185</v>
       </c>
       <c r="D118" s="18" t="s">
-        <v>187</v>
+        <v>506</v>
       </c>
       <c r="E118" s="18"/>
       <c r="F118" s="18" t="s">
@@ -6323,8 +6763,8 @@
       <c r="C119" s="5" t="s">
         <v>185</v>
       </c>
-      <c r="D119" s="5" t="s">
-        <v>187</v>
+      <c r="D119" s="18" t="s">
+        <v>507</v>
       </c>
       <c r="E119" s="5"/>
       <c r="F119" s="5" t="s">
@@ -6433,8 +6873,8 @@
       <c r="C123" s="36" t="s">
         <v>262</v>
       </c>
-      <c r="D123" s="15" t="s">
-        <v>267</v>
+      <c r="D123" s="36" t="s">
+        <v>489</v>
       </c>
       <c r="E123" s="15" t="s">
         <v>268</v>
@@ -6469,7 +6909,7 @@
         <v>371</v>
       </c>
       <c r="D124" s="18" t="s">
-        <v>267</v>
+        <v>490</v>
       </c>
       <c r="E124" s="15" t="s">
         <v>268</v>
@@ -8094,7 +8534,7 @@
         <v>262</v>
       </c>
       <c r="D179" s="37" t="s">
-        <v>263</v>
+        <v>491</v>
       </c>
       <c r="E179" s="37" t="s">
         <v>265</v>
@@ -8129,7 +8569,7 @@
         <v>274</v>
       </c>
       <c r="D180" s="37" t="s">
-        <v>263</v>
+        <v>491</v>
       </c>
       <c r="E180" s="37" t="s">
         <v>265</v>
@@ -8164,7 +8604,7 @@
         <v>371</v>
       </c>
       <c r="D181" s="18" t="s">
-        <v>263</v>
+        <v>492</v>
       </c>
       <c r="E181" s="35" t="s">
         <v>265</v>
@@ -8199,7 +8639,7 @@
         <v>262</v>
       </c>
       <c r="D182" s="37" t="s">
-        <v>264</v>
+        <v>493</v>
       </c>
       <c r="E182" s="37" t="s">
         <v>266</v>
@@ -8234,7 +8674,7 @@
         <v>274</v>
       </c>
       <c r="D183" s="37" t="s">
-        <v>264</v>
+        <v>493</v>
       </c>
       <c r="E183" s="37" t="s">
         <v>266</v>
@@ -8269,7 +8709,7 @@
         <v>371</v>
       </c>
       <c r="D184" s="18" t="s">
-        <v>264</v>
+        <v>494</v>
       </c>
       <c r="E184" s="18" t="s">
         <v>266</v>
@@ -9002,7 +9442,7 @@
       </c>
       <c r="C209" s="34"/>
       <c r="D209" s="34" t="s">
-        <v>357</v>
+        <v>508</v>
       </c>
       <c r="E209" s="34" t="s">
         <v>225</v>
@@ -9025,7 +9465,7 @@
       </c>
       <c r="C210" s="34"/>
       <c r="D210" s="34" t="s">
-        <v>357</v>
+        <v>509</v>
       </c>
       <c r="E210" s="34" t="s">
         <v>225</v>
@@ -10675,7 +11115,7 @@
       </c>
       <c r="C266" s="18"/>
       <c r="D266" s="18" t="s">
-        <v>181</v>
+        <v>510</v>
       </c>
       <c r="E266" s="18"/>
       <c r="F266" s="18" t="s">
@@ -10700,7 +11140,7 @@
       </c>
       <c r="C267" s="18"/>
       <c r="D267" s="18" t="s">
-        <v>181</v>
+        <v>511</v>
       </c>
       <c r="E267" s="18"/>
       <c r="F267" s="18" t="s">
@@ -10725,7 +11165,7 @@
       </c>
       <c r="C268" s="18"/>
       <c r="D268" s="18" t="s">
-        <v>181</v>
+        <v>512</v>
       </c>
       <c r="E268" s="18"/>
       <c r="F268" s="18" t="s">
@@ -10750,7 +11190,7 @@
       </c>
       <c r="C269" s="18"/>
       <c r="D269" s="18" t="s">
-        <v>181</v>
+        <v>513</v>
       </c>
       <c r="E269" s="18"/>
       <c r="F269" s="18" t="s">
@@ -10775,7 +11215,7 @@
       </c>
       <c r="C270" s="18"/>
       <c r="D270" s="18" t="s">
-        <v>181</v>
+        <v>416</v>
       </c>
       <c r="E270" s="18"/>
       <c r="F270" s="18" t="s">
@@ -10800,7 +11240,7 @@
       </c>
       <c r="C271" s="18"/>
       <c r="D271" s="18" t="s">
-        <v>181</v>
+        <v>514</v>
       </c>
       <c r="E271" s="18"/>
       <c r="F271" s="18" t="s">
@@ -10927,7 +11367,7 @@
         <v>221</v>
       </c>
       <c r="D276" s="53" t="s">
-        <v>416</v>
+        <v>515</v>
       </c>
       <c r="E276" s="24"/>
       <c r="F276" s="55"/>
@@ -32433,31 +32873,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="56" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="56" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="56" t="s">
+      <c r="A1" s="58" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="58" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="58" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="56" t="s">
+      <c r="D1" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="56" t="s">
+      <c r="E1" s="58" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="56" t="s">
+      <c r="F1" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="56" t="s">
+      <c r="G1" s="58" t="s">
         <v>208</v>
       </c>
       <c r="H1" s="25" t="s">
         <v>313</v>
       </c>
-      <c r="I1" s="58" t="s">
+      <c r="I1" s="60" t="s">
         <v>146</v>
       </c>
       <c r="J1" s="25" t="s">
@@ -32468,17 +32908,17 @@
       </c>
     </row>
     <row r="2" spans="1:11">
-      <c r="A2" s="57"/>
-      <c r="B2" s="57"/>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57"/>
-      <c r="F2" s="57"/>
-      <c r="G2" s="57"/>
+      <c r="A2" s="59"/>
+      <c r="B2" s="59"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="59"/>
       <c r="H2" s="26" t="s">
         <v>314</v>
       </c>
-      <c r="I2" s="59"/>
+      <c r="I2" s="61"/>
       <c r="J2" s="26" t="s">
         <v>314</v>
       </c>

</xml_diff>